<commit_message>
Merge request from "Concept improvement"
</commit_message>
<xml_diff>
--- a/documentation/timemanagment/beyer-timemanagement.xlsx
+++ b/documentation/timemanagment/beyer-timemanagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Martin\uibk\4th\SoftwareEngineering\g6t3\documentation\timemanagment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F55E99-40B4-4687-A181-CE917FF431E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA30986-C6CA-4A4B-A15D-60302AACBFEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
   <si>
     <t>Datum</t>
   </si>
@@ -264,6 +264,24 @@
   </si>
   <si>
     <t>Final Test v2. Docker Bugs (busy wait)</t>
+  </si>
+  <si>
+    <t>Helping other team</t>
+  </si>
+  <si>
+    <t>1 First look at other system</t>
+  </si>
+  <si>
+    <t>Problems with pi install + getting help from other team</t>
+  </si>
+  <si>
+    <t>Writing the feedback</t>
+  </si>
+  <si>
+    <t>Feedback annehmen</t>
+  </si>
+  <si>
+    <t>Feedback verwalten -&gt; Issues erstellen</t>
   </si>
 </sst>
 </file>
@@ -345,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -362,6 +380,7 @@
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,10 +698,10 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L55" sqref="L55"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -694,7 +713,7 @@
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="31.5">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="31.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -708,7 +727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="8">
         <v>44199</v>
       </c>
@@ -721,8 +740,9 @@
       <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="8">
         <v>44380</v>
       </c>
@@ -735,8 +755,9 @@
       <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="8">
         <v>44411</v>
       </c>
@@ -752,8 +773,9 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="8">
         <v>44533</v>
       </c>
@@ -767,8 +789,9 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="8">
         <v>44269</v>
       </c>
@@ -784,8 +807,9 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="8">
         <v>44271</v>
       </c>
@@ -801,8 +825,9 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="8">
         <v>44273</v>
       </c>
@@ -815,8 +840,9 @@
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="8">
         <v>44277</v>
       </c>
@@ -827,8 +853,9 @@
         <v>4</v>
       </c>
       <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="8">
         <v>44279</v>
       </c>
@@ -844,8 +871,9 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="8">
         <v>44280</v>
       </c>
@@ -858,8 +886,9 @@
       <c r="D11" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="8">
         <v>44282</v>
       </c>
@@ -872,8 +901,9 @@
       <c r="D12" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="8">
         <v>43918</v>
       </c>
@@ -886,8 +916,9 @@
       <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="8">
         <v>43920</v>
       </c>
@@ -900,8 +931,9 @@
       <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="8">
         <v>44287</v>
       </c>
@@ -914,8 +946,9 @@
       <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="8">
         <v>44288</v>
       </c>
@@ -928,6 +961,7 @@
       <c r="D16" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="8">
@@ -942,6 +976,7 @@
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="8">
@@ -956,6 +991,7 @@
       <c r="D18" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="8">
@@ -970,6 +1006,7 @@
       <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="8">
@@ -984,6 +1021,7 @@
       <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="8">
@@ -998,6 +1036,7 @@
       <c r="D21" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="8">
@@ -1014,7 +1053,7 @@
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="8">
@@ -1029,6 +1068,7 @@
       <c r="D23" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="8">
@@ -1043,6 +1083,7 @@
       <c r="D24" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="8">
@@ -1057,6 +1098,7 @@
       <c r="D25" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="8">
@@ -1071,6 +1113,7 @@
       <c r="D26" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="8">
@@ -1085,6 +1128,7 @@
       <c r="D27" s="10" t="s">
         <v>39</v>
       </c>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2">
@@ -1099,6 +1143,7 @@
       <c r="D28" s="10" t="s">
         <v>40</v>
       </c>
+      <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="8">
@@ -1113,6 +1158,7 @@
       <c r="D29" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="8">
@@ -1127,6 +1173,7 @@
       <c r="D30" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="8">
@@ -1141,6 +1188,7 @@
       <c r="D31" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="8">
@@ -1155,6 +1203,7 @@
       <c r="D32" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="8">
@@ -1169,6 +1218,7 @@
       <c r="D33" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="8">
@@ -1183,6 +1233,7 @@
       <c r="D34" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="8">
@@ -1197,6 +1248,7 @@
       <c r="D35" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="8">
@@ -1211,6 +1263,7 @@
       <c r="D36" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="8">
@@ -1225,6 +1278,7 @@
       <c r="D37" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="8">
@@ -1239,6 +1293,7 @@
       <c r="D38" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="8">
@@ -1253,6 +1308,7 @@
       <c r="D39" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="8">
@@ -1267,6 +1323,7 @@
       <c r="D40" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="8">
@@ -1281,6 +1338,7 @@
       <c r="D41" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="8">
@@ -1295,6 +1353,7 @@
       <c r="D42" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="H42" s="12"/>
       <c r="J42" s="11"/>
     </row>
     <row r="43" spans="1:14">
@@ -1310,6 +1369,7 @@
       <c r="D43" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="H43" s="12"/>
       <c r="J43" s="11"/>
     </row>
     <row r="44" spans="1:14">
@@ -1325,6 +1385,7 @@
       <c r="D44" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="H44" s="12"/>
       <c r="J44" s="11"/>
     </row>
     <row r="45" spans="1:14">
@@ -1340,6 +1401,7 @@
       <c r="D45" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="H45" s="12"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
@@ -1357,6 +1419,7 @@
       <c r="D46" s="3" t="s">
         <v>57</v>
       </c>
+      <c r="H46" s="12"/>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
@@ -1375,6 +1438,7 @@
       <c r="D47" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="H47" s="12"/>
       <c r="N47" s="7"/>
     </row>
     <row r="48" spans="1:14">
@@ -1390,6 +1454,7 @@
       <c r="D48" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="H48" s="12"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
@@ -1408,6 +1473,7 @@
       <c r="D49" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="H49" s="12"/>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="8">
@@ -1422,6 +1488,7 @@
       <c r="D50" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="H50" s="12"/>
       <c r="J50" s="7"/>
     </row>
     <row r="51" spans="1:11">
@@ -1437,6 +1504,7 @@
       <c r="D51" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="H51" s="12"/>
       <c r="J51" s="7"/>
     </row>
     <row r="52" spans="1:11">
@@ -1452,6 +1520,7 @@
       <c r="D52" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="H52" s="12"/>
       <c r="J52" s="7"/>
     </row>
     <row r="53" spans="1:11">
@@ -1467,6 +1536,7 @@
       <c r="D53" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="H53" s="12"/>
       <c r="J53" s="7"/>
     </row>
     <row r="54" spans="1:11">
@@ -1482,6 +1552,7 @@
       <c r="D54" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="H54" s="12"/>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="8">
@@ -1496,7 +1567,7 @@
       <c r="D55" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H55" s="7"/>
+      <c r="H55" s="12"/>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="8">
@@ -1511,7 +1582,7 @@
       <c r="D56" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H56" s="7"/>
+      <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="8">
@@ -1526,7 +1597,7 @@
       <c r="D57" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H57" s="7"/>
+      <c r="H57" s="12"/>
       <c r="J57" s="7"/>
     </row>
     <row r="58" spans="1:11">
@@ -1540,6 +1611,7 @@
         <v>4</v>
       </c>
       <c r="D58" s="3"/>
+      <c r="H58" s="12"/>
       <c r="J58" s="7"/>
     </row>
     <row r="59" spans="1:11">
@@ -1555,6 +1627,7 @@
       <c r="D59" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="H59" s="12"/>
       <c r="J59" s="7"/>
     </row>
     <row r="60" spans="1:11">
@@ -1570,6 +1643,7 @@
       <c r="D60" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="H60" s="12"/>
       <c r="K60" s="9"/>
     </row>
     <row r="61" spans="1:11">
@@ -1585,6 +1659,7 @@
       <c r="D61" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="H61" s="12"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
     </row>
@@ -1601,6 +1676,7 @@
       <c r="D62" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="H62" s="12"/>
       <c r="K62" s="9"/>
     </row>
     <row r="63" spans="1:11">
@@ -1616,6 +1692,7 @@
       <c r="D63" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="8">
@@ -1630,83 +1707,145 @@
       <c r="D64" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="8"/>
-      <c r="B65" s="7"/>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="8"/>
-      <c r="B66" s="7"/>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="8"/>
-      <c r="B67" s="7"/>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="8"/>
-      <c r="B68" s="7"/>
-      <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="8"/>
-      <c r="B69" s="7"/>
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="8"/>
-      <c r="B70" s="7"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="H64" s="12"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="8">
+        <v>44333</v>
+      </c>
+      <c r="B65" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H65" s="12"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="8">
+        <v>44334</v>
+      </c>
+      <c r="B66" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H66" s="12"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="8">
+        <v>44334</v>
+      </c>
+      <c r="B67" s="7">
+        <v>0.1423611111111111</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H67" s="12"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="8">
+        <v>44335</v>
+      </c>
+      <c r="B68" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H68" s="12"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="8">
+        <v>44340</v>
+      </c>
+      <c r="B69" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H69" s="12"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="8">
+        <v>44344</v>
+      </c>
+      <c r="B70" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H70" s="12"/>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="8"/>
       <c r="B71" s="7"/>
       <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="H71" s="12"/>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="8"/>
       <c r="B72" s="7"/>
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:8">
       <c r="A73" s="8"/>
       <c r="B73" s="7"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:8">
       <c r="A74" s="8"/>
       <c r="B74" s="7"/>
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:8">
       <c r="A75" s="8"/>
       <c r="B75" s="7"/>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:8">
       <c r="A76" s="8"/>
       <c r="B76" s="7"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:8">
       <c r="A77" s="8"/>
       <c r="B77" s="7"/>
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:8">
       <c r="A78" s="8"/>
       <c r="B78" s="7"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:8">
       <c r="A79" s="8"/>
       <c r="B79" s="7"/>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:8">
       <c r="A80" s="8"/>
       <c r="B80" s="7"/>
       <c r="D80" s="3"/>
@@ -6314,7 +6453,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4555F9B-702D-FD4F-A0B2-5CBE96A3F479}">
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>

</xml_diff>